<commit_message>
Izmjena scenarija za kupovinu
</commit_message>
<xml_diff>
--- a/UseCaseIScenarij/scenarij - kupovina.xlsx
+++ b/UseCaseIScenarij/scenarij - kupovina.xlsx
@@ -75,9 +75,6 @@
     <t>5. Kupovina nije uspješna zbog neispravnosti podataka</t>
   </si>
   <si>
-    <t>3. Popunjavanje osobnih podataka i podataka o plaćanju</t>
-  </si>
-  <si>
     <t>Kupac vrši pregled dostupnih knjiga, bira knjigu koja mu se dopada, zatim popunjava osobne podatke i informacije o plaćanju</t>
   </si>
   <si>
@@ -91,6 +88,9 @@
   </si>
   <si>
     <t>Kupac se prijavljuje na račun, zatim iz kataloga dostupnih knjiga bira željenu knjigu. Nakon toga, popunjava osobne podatke i informacije o plaćanju.</t>
+  </si>
+  <si>
+    <t>3. Popunjavanje podataka o plaćanju</t>
   </si>
 </sst>
 </file>
@@ -407,6 +407,30 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -433,30 +457,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -785,7 +785,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -793,7 +793,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -801,7 +801,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -809,7 +809,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -821,15 +821,15 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="29" t="s">
+      <c r="A7" s="17" t="s">
         <v>9</v>
       </c>
       <c r="B7" s="5"/>
     </row>
     <row r="8" spans="1:3" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="30"/>
+      <c r="A8" s="18"/>
       <c r="B8" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
@@ -844,112 +844,112 @@
       <c r="A11" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="31" t="s">
+      <c r="B11" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="32"/>
+      <c r="C11" s="20"/>
     </row>
     <row r="12" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="25"/>
-      <c r="C12" s="26"/>
+      <c r="B12" s="21"/>
+      <c r="C12" s="22"/>
     </row>
     <row r="13" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="25"/>
-      <c r="C13" s="26"/>
+      <c r="B13" s="21"/>
+      <c r="C13" s="22"/>
     </row>
     <row r="14" spans="1:3" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="B14" s="25"/>
-      <c r="C14" s="26"/>
+        <v>24</v>
+      </c>
+      <c r="B14" s="21"/>
+      <c r="C14" s="22"/>
     </row>
     <row r="15" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="11"/>
-      <c r="B15" s="27" t="s">
+      <c r="B15" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="28"/>
+      <c r="C15" s="16"/>
     </row>
     <row r="16" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="12"/>
-      <c r="B16" s="15" t="s">
+      <c r="B16" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="16"/>
+      <c r="C16" s="24"/>
     </row>
     <row r="17" spans="1:3" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="17"/>
-      <c r="C17" s="17"/>
+      <c r="B17" s="25"/>
+      <c r="C17" s="25"/>
     </row>
     <row r="18" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A18" s="8"/>
-      <c r="B18" s="18"/>
-      <c r="C18" s="18"/>
+      <c r="B18" s="26"/>
+      <c r="C18" s="26"/>
     </row>
     <row r="19" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A19" s="19" t="s">
+      <c r="A19" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="B19" s="19"/>
-      <c r="C19" s="21"/>
+      <c r="B19" s="27"/>
+      <c r="C19" s="29"/>
     </row>
     <row r="20" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="20" t="s">
+      <c r="A20" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="B20" s="20"/>
-      <c r="C20" s="22"/>
+      <c r="B20" s="28"/>
+      <c r="C20" s="30"/>
     </row>
     <row r="21" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="B21" s="23" t="s">
+      <c r="B21" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="C21" s="24"/>
+      <c r="C21" s="32"/>
     </row>
     <row r="22" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="B22" s="25"/>
-      <c r="C22" s="26"/>
+      <c r="B22" s="21"/>
+      <c r="C22" s="22"/>
     </row>
     <row r="23" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B23" s="25"/>
-      <c r="C23" s="26"/>
+      <c r="B23" s="21"/>
+      <c r="C23" s="22"/>
     </row>
     <row r="24" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="B24" s="25"/>
-      <c r="C24" s="26"/>
+        <v>24</v>
+      </c>
+      <c r="B24" s="21"/>
+      <c r="C24" s="22"/>
     </row>
     <row r="25" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="11"/>
-      <c r="B25" s="27" t="s">
+      <c r="B25" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="C25" s="28"/>
+      <c r="C25" s="16"/>
     </row>
     <row r="26" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="12"/>
-      <c r="B26" s="15" t="s">
+      <c r="B26" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="C26" s="16"/>
+      <c r="C26" s="24"/>
     </row>
     <row r="27" spans="1:3" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A27" s="13"/>
@@ -961,12 +961,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B14:C14"/>
     <mergeCell ref="B26:C26"/>
     <mergeCell ref="B16:C16"/>
     <mergeCell ref="B17:C17"/>
@@ -979,6 +973,12 @@
     <mergeCell ref="B23:C23"/>
     <mergeCell ref="B24:C24"/>
     <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B14:C14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>